<commit_message>
Updates to mapping; temporary fix for publication author parsing
</commit_message>
<xml_diff>
--- a/data/to-migrate/mapping/Teaching Activities Choice Lists.xlsx
+++ b/data/to-migrate/mapping/Teaching Activities Choice Lists.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsmith/Documents/code/lyterati-elements/data/to-migrate/mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E44A376-380A-2C4D-92C7-B044B5E5BE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF2C986-F052-FE40-A557-D8CACC38384B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{0A719D6D-1F6B-C84B-89C8-9C7DB8739AF5}"/>
+    <workbookView xWindow="-28220" yWindow="1960" windowWidth="28040" windowHeight="15820" xr2:uid="{0A719D6D-1F6B-C84B-89C8-9C7DB8739AF5}"/>
   </bookViews>
   <sheets>
     <sheet name="degree-type" sheetId="1" r:id="rId1"/>
+    <sheet name="c-placement-type" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Elements</t>
   </si>
@@ -65,9 +66,6 @@
     <t>Clinical</t>
   </si>
   <si>
-    <t>Docotr (other health professions)</t>
-  </si>
-  <si>
     <t>Doctorate</t>
   </si>
   <si>
@@ -96,13 +94,28 @@
   </si>
   <si>
     <t>Registered Nurse</t>
+  </si>
+  <si>
+    <t>Academic</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Doctor (other health professions)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,6 +124,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -137,9 +158,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +499,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,57 +548,112 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63BFE6F-2E23-2B4E-BB3F-A32F53ED76C8}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>